<commit_message>
update operation test excel
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/OperationTest2007.xlsx
+++ b/zss.test/src/main/webapp/OperationTest2007.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12225" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cell-text" sheetId="4" r:id="rId1"/>
+    <sheet name="cell" sheetId="4" r:id="rId1"/>
     <sheet name="cell-border" sheetId="5" r:id="rId2"/>
     <sheet name="cell-data" sheetId="6" r:id="rId3"/>
     <sheet name="row" sheetId="1" r:id="rId4"/>
     <sheet name="chart-image" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
+    <sheet name="blank" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
@@ -81,12 +81,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+(Help) Fill data automatically in worksheet cells</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>copy</t>
   </si>
@@ -305,26 +329,59 @@
     <t>vertical</t>
   </si>
   <si>
-    <t>horizontal</t>
-  </si>
-  <si>
     <t>item 1</t>
   </si>
   <si>
     <t>item 2</t>
   </si>
   <si>
-    <t>include text</t>
-  </si>
-  <si>
     <t>drag move</t>
+  </si>
+  <si>
+    <t>numbers</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Week Day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>1st period</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>text with Number</t>
+  </si>
+  <si>
+    <t>3 cells</t>
+  </si>
+  <si>
+    <t>clear style</t>
+  </si>
+  <si>
+    <t>of these</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +455,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -480,7 +544,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -492,20 +556,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,6 +573,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -554,7 +624,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:rotX val="30"/>
@@ -657,7 +726,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -677,10 +746,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121903"/>
+          <c:x val="0.1578974953712193"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700539"/>
-          <c:h val="0.76578566465956821"/>
+          <c:w val="0.58796850393700473"/>
+          <c:h val="0.76578566465956921"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -907,25 +976,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134853376"/>
-        <c:axId val="134854912"/>
-        <c:axId val="134857152"/>
+        <c:axId val="92133248"/>
+        <c:axId val="92134784"/>
+        <c:axId val="92079424"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="134853376"/>
+        <c:axId val="92133248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134854912"/>
+        <c:crossAx val="92134784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134854912"/>
+        <c:axId val="92134784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,24 +1002,23 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134853376"/>
+        <c:crossAx val="92133248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="134857152"/>
+        <c:axId val="92079424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134854912"/>
+        <c:crossAx val="92134784"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -959,7 +1027,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1210,22 +1278,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="135872896"/>
-        <c:axId val="135874432"/>
+        <c:axId val="92177920"/>
+        <c:axId val="92179456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135872896"/>
+        <c:axId val="92177920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135874432"/>
+        <c:crossAx val="92179456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135874432"/>
+        <c:axId val="92179456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,20 +1301,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135872896"/>
+        <c:crossAx val="92177920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1503,288 +1570,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Internet Explorer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$B$14:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.3427</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.32700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.31680000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.30809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.28870000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28949999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.28489999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$C$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Chrome</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$C$14:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.25990000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28089999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.28239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.29149999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.29349999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.30059999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$D$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$D$14:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.2268</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2276</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2273</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.22489999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.22969999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.21010000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="155165440"/>
-        <c:axId val="155167360"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="155165440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155167360"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="155167360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155165440"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1810,7 +1601,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1884,8 +1674,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479912"/>
-          <c:h val="0.56509104330708892"/>
+          <c:w val="0.25885988970479945"/>
+          <c:h val="0.5650910433070897"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1904,7 +1694,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2141,24 +1931,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="137179904"/>
-        <c:axId val="137181440"/>
+        <c:axId val="90782336"/>
+        <c:axId val="90788224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137179904"/>
+        <c:axId val="90782336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137181440"/>
+        <c:crossAx val="90788224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137181440"/>
+        <c:axId val="90788224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,20 +1956,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137179904"/>
+        <c:crossAx val="90782336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2420,25 +2209,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="137211264"/>
-        <c:axId val="137221248"/>
+        <c:axId val="90801664"/>
+        <c:axId val="90803200"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="137211264"/>
+        <c:axId val="90801664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137221248"/>
+        <c:crossAx val="90803200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137221248"/>
+        <c:axId val="90803200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2446,20 +2235,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137211264"/>
+        <c:crossAx val="90801664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2705,24 +2493,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="111417216"/>
-        <c:axId val="111418752"/>
+        <c:axId val="91422720"/>
+        <c:axId val="91424256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111417216"/>
+        <c:axId val="91422720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111418752"/>
+        <c:crossAx val="91424256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111418752"/>
+        <c:axId val="91424256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2730,7 +2518,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111417216"/>
+        <c:crossAx val="91422720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2742,7 +2530,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2981,25 +2769,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="111477504"/>
-        <c:axId val="111479040"/>
-        <c:axId val="137218688"/>
+        <c:axId val="91462272"/>
+        <c:axId val="91468160"/>
+        <c:axId val="91443200"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="111477504"/>
+        <c:axId val="91462272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111479040"/>
+        <c:crossAx val="91468160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111479040"/>
+        <c:axId val="91468160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3007,19 +2795,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111477504"/>
+        <c:crossAx val="91462272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="137218688"/>
+        <c:axId val="91443200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="111479040"/>
+        <c:crossAx val="91468160"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3030,7 +2818,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3267,24 +3055,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="111538560"/>
-        <c:axId val="111540096"/>
+        <c:axId val="91490560"/>
+        <c:axId val="91504640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111538560"/>
+        <c:axId val="91490560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111540096"/>
+        <c:crossAx val="91504640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111540096"/>
+        <c:axId val="91504640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3292,7 +3080,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111538560"/>
+        <c:crossAx val="91490560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3304,7 +3092,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3326,7 +3114,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.503213971867704"/>
+          <c:w val="0.503213971867703"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -3556,25 +3344,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="113073152"/>
-        <c:axId val="113079040"/>
+        <c:axId val="91543040"/>
+        <c:axId val="91544576"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113073152"/>
+        <c:axId val="91543040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113079040"/>
+        <c:crossAx val="91544576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113079040"/>
+        <c:axId val="91544576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,14 +3370,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113073152"/>
+        <c:crossAx val="91543040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3598,7 +3385,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3834,24 +3621,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="113100672"/>
-        <c:axId val="113102208"/>
+        <c:axId val="91553152"/>
+        <c:axId val="92091520"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="113100672"/>
+        <c:axId val="91553152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113102208"/>
+        <c:crossAx val="92091520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113102208"/>
+        <c:axId val="92091520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3859,20 +3646,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113100672"/>
+        <c:crossAx val="91553152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4285,79 +4071,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="highlight_banner_essentials.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3048000" y="1143000"/>
-          <a:ext cx="2619375" cy="904875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -4702,10 +4415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H49"/>
+  <dimension ref="A2:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4714,24 +4427,24 @@
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="21">
+    <row r="2" spans="1:9" ht="21">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="21">
+    <row r="3" spans="1:9" ht="21">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="21">
+    <row r="4" spans="1:9" ht="23.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="20">
         <f>SUM(D4:F4)</f>
         <v>6</v>
       </c>
@@ -4745,8 +4458,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="42">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:9" ht="42">
+      <c r="A5" s="16" t="s">
         <v>68</v>
       </c>
       <c r="B5">
@@ -4763,28 +4476,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="42">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:9" ht="42">
+      <c r="A6" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21">
-      <c r="A7" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:9" ht="21">
+      <c r="A7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" ht="21">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" ht="21">
       <c r="A8" s="1"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="21">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="21">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>4</v>
@@ -4792,48 +4505,98 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="11"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="11" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="3"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="21">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="21">
       <c r="A17" s="1"/>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="C17" s="21"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="21">
+    <row r="20" spans="1:9">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="21">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21">
+    <row r="23" spans="1:9" ht="21">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4845,178 +4608,237 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21">
+    <row r="24" spans="1:9" ht="21">
       <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" ht="21">
+      <c r="A25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="21">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="21">
+      <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="18">
+        <v>2007</v>
+      </c>
+      <c r="C27" s="18">
+        <v>2008</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" ht="21">
+      <c r="A28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" ht="21">
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="21">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="30" spans="1:9" ht="21">
+      <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B25">
+      <c r="B30">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21">
-      <c r="A26" s="1"/>
-      <c r="B26">
+    <row r="31" spans="1:9" ht="21">
+      <c r="A31" s="1"/>
+      <c r="B31">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="33" spans="1:8" ht="21">
-      <c r="A33" s="1" t="s">
+    <row r="32" spans="1:9" ht="21">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="21">
+      <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33">
-        <f>SUM(D33:E33)</f>
+      <c r="C38">
+        <f>SUM(D38:E38)</f>
         <v>2</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="E33">
+      <c r="E38">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="21">
-      <c r="A34" s="1"/>
-      <c r="D34">
+    <row r="39" spans="1:5" ht="21">
+      <c r="A39" s="1"/>
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E34">
+      <c r="E39">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="21">
-      <c r="A35" s="1"/>
-      <c r="D35">
+    <row r="40" spans="1:5" ht="21">
+      <c r="A40" s="1"/>
+      <c r="D40">
         <v>3</v>
       </c>
-      <c r="E35">
+      <c r="E40">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="21">
-      <c r="A36" s="1"/>
-      <c r="D36">
+    <row r="41" spans="1:5" ht="21">
+      <c r="A41" s="1"/>
+      <c r="D41">
         <v>4</v>
       </c>
-      <c r="E36">
+      <c r="E41">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="21">
-      <c r="A37" s="1"/>
-      <c r="D37">
+    <row r="42" spans="1:5" ht="21">
+      <c r="A42" s="1"/>
+      <c r="D42">
         <v>5</v>
       </c>
-      <c r="E37">
+      <c r="E42">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="21">
-      <c r="A38" s="1"/>
-      <c r="D38">
+    <row r="43" spans="1:5" ht="21">
+      <c r="A43" s="1"/>
+      <c r="D43">
         <v>6</v>
       </c>
-      <c r="E38">
+      <c r="E43">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="21">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" ht="21">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" ht="21">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="44" spans="1:8" ht="21">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" ht="21">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="21">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="21">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="49" spans="1:8" ht="21">
+      <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B49" t="s">
         <v>65</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E49" t="s">
         <v>66</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H49" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="18.75">
-      <c r="B45" s="18">
+    <row r="50" spans="1:8" ht="18.75">
+      <c r="B50" s="15">
         <v>5</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E50" s="2">
         <v>2</v>
       </c>
-      <c r="F45" s="2"/>
-      <c r="H45">
+      <c r="F50" s="2"/>
+      <c r="H50">
         <f>SUM(1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="18.75">
-      <c r="B46" s="18">
+    <row r="51" spans="1:8" ht="18.75">
+      <c r="B51" s="15">
         <v>3</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E51" s="2">
         <v>3</v>
       </c>
-      <c r="F46" s="2"/>
-      <c r="H46">
+      <c r="F51" s="2"/>
+      <c r="H51">
         <f>SUM(2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18.75">
-      <c r="B47" s="18">
+    <row r="52" spans="1:8" ht="18.75">
+      <c r="B52" s="15">
         <v>1</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E52" s="2">
         <v>1</v>
       </c>
-      <c r="F47" s="2"/>
-      <c r="H47">
+      <c r="F52" s="2"/>
+      <c r="H52">
         <f>SUM(3)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="18.75">
-      <c r="B48" s="18">
+    <row r="53" spans="1:8" ht="18.75">
+      <c r="B53" s="15">
         <v>4</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E53" s="2">
         <v>4</v>
       </c>
-      <c r="F48" s="2"/>
-      <c r="H48">
+      <c r="F53" s="2"/>
+      <c r="H53">
         <f>SUM(4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="18.75">
-      <c r="B49" s="18">
+    <row r="54" spans="1:8" ht="18.75">
+      <c r="B54" s="15">
         <v>2</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E54" s="2">
         <v>5</v>
       </c>
-      <c r="F49" s="2"/>
-      <c r="H49">
+      <c r="F54" s="2"/>
+      <c r="H54">
         <f>SUM(5)</f>
         <v>5</v>
       </c>
@@ -5040,10 +4862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5083,26 +4905,26 @@
       <c r="F3" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="7"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="7"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
@@ -5136,14 +4958,14 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:8" ht="45">
       <c r="B21" s="4" t="s">
@@ -5151,7 +4973,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B25" t="s">
@@ -5166,8 +4988,32 @@
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="5"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5325,7 +5171,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="N12" t="s">
@@ -5333,16 +5179,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5350,13 +5196,13 @@
       <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>0.3427</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>0.25990000000000002</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>0.2268</v>
       </c>
     </row>
@@ -5364,13 +5210,13 @@
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <v>0.32700000000000001</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>0.27239999999999998</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>0.2276</v>
       </c>
     </row>
@@ -5378,13 +5224,13 @@
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <v>0.31680000000000003</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>0.28089999999999998</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>0.2273</v>
       </c>
     </row>
@@ -5392,13 +5238,13 @@
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <v>0.30809999999999998</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>0.28239999999999998</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>0.22489999999999999</v>
       </c>
     </row>
@@ -5406,13 +5252,13 @@
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <v>0.28870000000000001</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>0.29149999999999998</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>0.22969999999999999</v>
       </c>
     </row>
@@ -5420,13 +5266,13 @@
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <v>0.28949999999999998</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>0.29349999999999998</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>0.22</v>
       </c>
     </row>
@@ -5434,13 +5280,13 @@
       <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <v>0.28489999999999999</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>0.30059999999999998</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>0.21010000000000001</v>
       </c>
     </row>
@@ -5448,13 +5294,13 @@
       <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="12">
         <v>0.2898</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="12">
         <v>0.29630000000000001</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>0.2016</v>
       </c>
     </row>
@@ -5462,13 +5308,13 @@
       <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="12">
         <v>0.28770000000000001</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="12">
         <v>0.30009999999999998</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="12">
         <v>0.19700000000000001</v>
       </c>
     </row>
@@ -5476,13 +5322,13 @@
       <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>0.28129999999999999</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>0.3049</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>0.19570000000000001</v>
       </c>
     </row>
@@ -5490,13 +5336,13 @@
       <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="12">
         <v>0.27150000000000002</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="12">
         <v>0.3105</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="12">
         <v>0.19739999999999999</v>
       </c>
     </row>
@@ -5504,13 +5350,13 @@
       <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="12">
         <v>0.26300000000000001</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="12">
         <v>0.31119999999999998</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="12">
         <v>0.18709999999999999</v>
       </c>
     </row>
@@ -5518,13 +5364,13 @@
       <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="12">
         <v>0.26369999999999999</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="12">
         <v>0.31509999999999999</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="12">
         <v>0.18390000000000001</v>
       </c>
     </row>
@@ -5532,13 +5378,13 @@
       <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="12">
         <v>0.25540000000000002</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="12">
         <v>0.3196</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="12">
         <v>0.18279999999999999</v>
       </c>
     </row>
@@ -5546,18 +5392,18 @@
       <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="12">
         <v>0.25080000000000002</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="12">
         <v>0.32879999999999998</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="12">
         <v>0.17860000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="18.75">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D32" t="s">
@@ -5568,7 +5414,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5621,7 +5467,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="18.75">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5631,7 +5477,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="18.75">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5646,12 +5492,12 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="18.75">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="18.75">
-      <c r="A117" s="14" t="s">
+      <c r="A117" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5661,7 +5507,7 @@
       </c>
     </row>
     <row r="137" spans="1:1" ht="18.75">
-      <c r="A137" s="14" t="s">
+      <c r="A137" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5693,21 +5539,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A10"/>
+  <dimension ref="E9:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="10" spans="1:1">
-      <c r="A10">
-        <v>1</v>
-      </c>
+    <row r="9" spans="5:6">
+      <c r="E9" s="19"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor revise operation test excel file
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/OperationTest2007.xlsx
+++ b/zss.test/src/main/webapp/OperationTest2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12225" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cell" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,9 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cell-border'!$K$25:$K$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'cell-data'!$A$1:$A$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'cell-data'!$A$1:$C$12</definedName>
+    <definedName name="range1">cell!$C$45:$E$45</definedName>
+    <definedName name="range2">cell!$C$46:$E$47</definedName>
     <definedName name="RangeMerged">'[1]cell-data'!$F$12</definedName>
     <definedName name="TestRange1">'[1]cell-data'!$B$12:$D$13</definedName>
   </definedNames>
@@ -110,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
   <si>
     <t>copy</t>
   </si>
@@ -155,9 +157,6 @@
   </si>
   <si>
     <t>size 16 text</t>
-  </si>
-  <si>
-    <t>Header</t>
   </si>
   <si>
     <t>2 cells, and bottom border appears</t>
@@ -375,6 +374,60 @@
   </si>
   <si>
     <t>of these</t>
+  </si>
+  <si>
+    <t>1. select these 9 cells, merge across</t>
+  </si>
+  <si>
+    <t>3. unmerge</t>
+  </si>
+  <si>
+    <t>named range</t>
+  </si>
+  <si>
+    <t>header 2</t>
+  </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>header 3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>range1</t>
+  </si>
+  <si>
+    <t>range2</t>
+  </si>
+  <si>
+    <t>range3</t>
+  </si>
+  <si>
+    <t>2. merge cells</t>
   </si>
 </sst>
 </file>
@@ -464,7 +517,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +527,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,7 +603,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -580,6 +639,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -726,7 +786,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -746,10 +806,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1578974953712193"/>
+          <c:x val="0.15789749537121964"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700473"/>
-          <c:h val="0.76578566465956921"/>
+          <c:w val="0.58796850393700395"/>
+          <c:h val="0.76578566465957054"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -976,25 +1036,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="92133248"/>
-        <c:axId val="92134784"/>
-        <c:axId val="92079424"/>
+        <c:axId val="76871936"/>
+        <c:axId val="76939264"/>
+        <c:axId val="79141952"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="92133248"/>
+        <c:axId val="76871936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92134784"/>
+        <c:crossAx val="76939264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92134784"/>
+        <c:axId val="76939264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,18 +1062,18 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92133248"/>
+        <c:crossAx val="76871936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="92079424"/>
+        <c:axId val="79141952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92134784"/>
+        <c:crossAx val="76939264"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1027,7 +1087,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1278,22 +1338,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92177920"/>
-        <c:axId val="92179456"/>
+        <c:axId val="76961664"/>
+        <c:axId val="76963200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92177920"/>
+        <c:axId val="76961664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92179456"/>
+        <c:crossAx val="76963200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92179456"/>
+        <c:axId val="76963200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,7 +1361,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92177920"/>
+        <c:crossAx val="76961664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1313,7 +1373,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1575,7 +1635,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1674,8 +1734,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479945"/>
-          <c:h val="0.5650910433070897"/>
+          <c:w val="0.25885988970479984"/>
+          <c:h val="0.56509104330709048"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1694,7 +1754,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1931,24 +1991,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90782336"/>
-        <c:axId val="90788224"/>
+        <c:axId val="92002560"/>
+        <c:axId val="94437760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90782336"/>
+        <c:axId val="92002560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90788224"/>
+        <c:crossAx val="94437760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90788224"/>
+        <c:axId val="94437760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,7 +2016,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90782336"/>
+        <c:crossAx val="92002560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1968,7 +2028,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2209,25 +2269,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="90801664"/>
-        <c:axId val="90803200"/>
+        <c:axId val="94510464"/>
+        <c:axId val="94787072"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="90801664"/>
+        <c:axId val="94510464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90803200"/>
+        <c:crossAx val="94787072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90803200"/>
+        <c:axId val="94787072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2235,7 +2295,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90801664"/>
+        <c:crossAx val="94510464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2247,7 +2307,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2493,24 +2553,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91422720"/>
-        <c:axId val="91424256"/>
+        <c:axId val="100289536"/>
+        <c:axId val="100659968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91422720"/>
+        <c:axId val="100289536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91424256"/>
+        <c:crossAx val="100659968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91424256"/>
+        <c:axId val="100659968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2518,7 +2578,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91422720"/>
+        <c:crossAx val="100289536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2530,7 +2590,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2769,25 +2829,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91462272"/>
-        <c:axId val="91468160"/>
-        <c:axId val="91443200"/>
+        <c:axId val="76782208"/>
+        <c:axId val="76792192"/>
+        <c:axId val="77065280"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="91462272"/>
+        <c:axId val="76782208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91468160"/>
+        <c:crossAx val="76792192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91468160"/>
+        <c:axId val="76792192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,19 +2855,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91462272"/>
+        <c:crossAx val="76782208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="91443200"/>
+        <c:axId val="77065280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="91468160"/>
+        <c:crossAx val="76792192"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2818,7 +2878,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3055,24 +3115,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91490560"/>
-        <c:axId val="91504640"/>
+        <c:axId val="76806400"/>
+        <c:axId val="76808192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91490560"/>
+        <c:axId val="76806400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91504640"/>
+        <c:crossAx val="76808192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91504640"/>
+        <c:axId val="76808192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3080,7 +3140,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91490560"/>
+        <c:crossAx val="76806400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3092,7 +3152,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3114,7 +3174,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.503213971867703"/>
+          <c:w val="0.50321397186770178"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -3344,25 +3404,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="91543040"/>
-        <c:axId val="91544576"/>
+        <c:axId val="76817920"/>
+        <c:axId val="76819456"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="91543040"/>
+        <c:axId val="76817920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91544576"/>
+        <c:crossAx val="76819456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91544576"/>
+        <c:axId val="76819456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3370,7 +3430,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91543040"/>
+        <c:crossAx val="76817920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3385,7 +3445,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3621,24 +3681,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91553152"/>
-        <c:axId val="92091520"/>
+        <c:axId val="76832768"/>
+        <c:axId val="76834304"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="91553152"/>
+        <c:axId val="76832768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92091520"/>
+        <c:crossAx val="76834304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92091520"/>
+        <c:axId val="76834304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3646,7 +3706,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91553152"/>
+        <c:crossAx val="76832768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3658,7 +3718,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4415,10 +4475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I54"/>
+  <dimension ref="A2:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4460,7 +4520,7 @@
     </row>
     <row r="5" spans="1:9" ht="42">
       <c r="A5" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <f>SUM(D5,E5,F5)</f>
@@ -4478,18 +4538,18 @@
     </row>
     <row r="6" spans="1:9" ht="42">
       <c r="A6" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21">
       <c r="A7" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:9" ht="21">
       <c r="A8" s="1"/>
@@ -4561,7 +4621,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -4573,10 +4633,10 @@
     </row>
     <row r="17" spans="1:9" ht="21">
       <c r="A17" s="1"/>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -4591,12 +4651,12 @@
     </row>
     <row r="22" spans="1:9" ht="21">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="21">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4610,7 +4670,7 @@
     </row>
     <row r="24" spans="1:9" ht="21">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="17">
         <v>0.375</v>
@@ -4621,10 +4681,10 @@
     </row>
     <row r="25" spans="1:9" ht="21">
       <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -4632,10 +4692,10 @@
     </row>
     <row r="26" spans="1:9" ht="21">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -4643,7 +4703,7 @@
     </row>
     <row r="27" spans="1:9" ht="21">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="18">
         <v>2007</v>
@@ -4656,10 +4716,10 @@
     </row>
     <row r="28" spans="1:9" ht="21">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -4669,18 +4729,18 @@
     </row>
     <row r="29" spans="1:9" ht="21">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
         <v>72</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="21">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4697,7 +4757,7 @@
     </row>
     <row r="38" spans="1:5" ht="21">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38">
         <f>SUM(D38:E38)</f>
@@ -4759,86 +4819,179 @@
       <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="21">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="21">
       <c r="A46" s="1"/>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="21">
+      <c r="A47" s="1"/>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="21">
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="21">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" ht="21">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" ht="21">
+      <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="21">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" ht="21">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+    </row>
+    <row r="55" spans="1:8" ht="21">
+      <c r="A55" s="1"/>
+      <c r="B55" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+    </row>
+    <row r="56" spans="1:8" ht="21">
+      <c r="A56" s="1"/>
+      <c r="B56" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+    </row>
+    <row r="57" spans="1:8" ht="21">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" ht="21">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="61" spans="1:8" ht="21">
+      <c r="A61" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" t="s">
         <v>65</v>
       </c>
-      <c r="E49" t="s">
+      <c r="H61" t="s">
         <v>66</v>
       </c>
-      <c r="H49" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="18.75">
-      <c r="B50" s="15">
+    </row>
+    <row r="62" spans="1:8" ht="18.75">
+      <c r="B62" s="15">
         <v>5</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E62" s="2">
         <v>2</v>
       </c>
-      <c r="F50" s="2"/>
-      <c r="H50">
+      <c r="F62" s="2"/>
+      <c r="H62">
         <f>SUM(1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="18.75">
-      <c r="B51" s="15">
+    <row r="63" spans="1:8" ht="18.75">
+      <c r="B63" s="15">
         <v>3</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E63" s="2">
         <v>3</v>
       </c>
-      <c r="F51" s="2"/>
-      <c r="H51">
+      <c r="F63" s="2"/>
+      <c r="H63">
         <f>SUM(2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="18.75">
-      <c r="B52" s="15">
+    <row r="64" spans="1:8" ht="18.75">
+      <c r="B64" s="15">
         <v>1</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E64" s="2">
         <v>1</v>
       </c>
-      <c r="F52" s="2"/>
-      <c r="H52">
+      <c r="F64" s="2"/>
+      <c r="H64">
         <f>SUM(3)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="18.75">
-      <c r="B53" s="15">
+    <row r="65" spans="2:8" ht="18.75">
+      <c r="B65" s="15">
         <v>4</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E65" s="2">
         <v>4</v>
       </c>
-      <c r="F53" s="2"/>
-      <c r="H53">
+      <c r="F65" s="2"/>
+      <c r="H65">
         <f>SUM(4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="18.75">
-      <c r="B54" s="15">
+    <row r="66" spans="2:8" ht="18.75">
+      <c r="B66" s="15">
         <v>2</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E66" s="2">
         <v>5</v>
       </c>
-      <c r="F54" s="2"/>
-      <c r="H54">
+      <c r="F66" s="2"/>
+      <c r="H66">
         <f>SUM(5)</f>
         <v>5</v>
       </c>
@@ -4864,8 +5017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4905,26 +5058,26 @@
       <c r="F3" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="21" t="s">
-        <v>18</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="21"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
@@ -4959,28 +5112,28 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="45">
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -4993,27 +5146,21 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5022,102 +5169,343 @@
     <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" hidden="1">
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" hidden="1">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" hidden="1">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" hidden="1">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" hidden="1">
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" hidden="1">
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" hidden="1">
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" hidden="1">
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>3</v>
       </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A12">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5138,17 +5526,17 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>7.28</v>
@@ -5156,7 +5544,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>1.98</v>
@@ -5164,37 +5552,37 @@
     </row>
     <row r="10" spans="1:14" ht="21">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="19.5" thickBot="1">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
       <c r="A13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="D13" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="12">
         <v>0.3427</v>
@@ -5208,7 +5596,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="12">
         <v>0.32700000000000001</v>
@@ -5222,7 +5610,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="12">
         <v>0.31680000000000003</v>
@@ -5236,7 +5624,7 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="12">
         <v>0.30809999999999998</v>
@@ -5250,7 +5638,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="12">
         <v>0.28870000000000001</v>
@@ -5264,7 +5652,7 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="12">
         <v>0.28949999999999998</v>
@@ -5278,7 +5666,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="12">
         <v>0.28489999999999999</v>
@@ -5292,7 +5680,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="12">
         <v>0.2898</v>
@@ -5306,7 +5694,7 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="12">
         <v>0.28770000000000001</v>
@@ -5320,7 +5708,7 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="12">
         <v>0.28129999999999999</v>
@@ -5334,7 +5722,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="12">
         <v>0.27150000000000002</v>
@@ -5348,7 +5736,7 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="12">
         <v>0.26300000000000001</v>
@@ -5362,7 +5750,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="12">
         <v>0.26369999999999999</v>
@@ -5376,7 +5764,7 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="12">
         <v>0.25540000000000002</v>
@@ -5390,7 +5778,7 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="12">
         <v>0.25080000000000002</v>
@@ -5404,23 +5792,23 @@
     </row>
     <row r="32" spans="1:12" ht="18.75">
       <c r="A32" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>44.6</v>
@@ -5428,7 +5816,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>22.08</v>
@@ -5436,7 +5824,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>18.170000000000002</v>
@@ -5444,7 +5832,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37">
         <v>9.07</v>
@@ -5452,7 +5840,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38">
         <v>3.38</v>
@@ -5460,7 +5848,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39">
         <v>3.24</v>
@@ -5468,47 +5856,47 @@
     </row>
     <row r="48" spans="1:2" ht="18.75">
       <c r="A48" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="12:12">
       <c r="L49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="18.75">
       <c r="A69" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="L70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="L94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="18.75">
       <c r="A95" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="18.75">
       <c r="A117" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="H120" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="18.75">
       <c r="A137" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="21">

</xml_diff>